<commit_message>
Backup + mise a jour timesheet + eleve vue début
</commit_message>
<xml_diff>
--- a/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
+++ b/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web2.0\Documents\2-UsersStories\Propre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1E3BBE-E761-4EF8-AFF6-57019D2F5CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E14F4AE-A93F-476F-AB81-9E938EBDEC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6BE69B5F-2B83-4C7C-919C-A491774D0366}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>Préparation</t>
   </si>
@@ -227,12 +227,6 @@
     <t>connexion DB</t>
   </si>
   <si>
-    <t>1h30</t>
-  </si>
-  <si>
-    <t>1h00</t>
-  </si>
-  <si>
     <t>redirection</t>
   </si>
   <si>
@@ -246,6 +240,21 @@
   </si>
   <si>
     <t>Avec style</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>2h30</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -274,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,12 +299,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,17 +330,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5B8967-943E-45FD-AD50-36B24B8571A1}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,14 +740,14 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -760,10 +762,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -778,14 +780,14 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -800,12 +802,12 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -818,11 +820,11 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -836,12 +838,12 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="7"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -854,164 +856,146 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>100</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>100</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>100</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>100</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>100</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>100</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>100</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1021,13 +1005,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1043,13 +1027,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1065,13 +1049,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1087,13 +1071,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1102,137 +1086,139 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
+      <c r="A23" s="1">
+        <v>100</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>100</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7" t="s">
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>80</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1241,18 +1227,20 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1261,13 +1249,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>25</v>
@@ -1283,13 +1271,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>26</v>
@@ -1303,13 +1291,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>45</v>
@@ -1322,11 +1310,21 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="1">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1334,10 +1332,18 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="A35" s="1">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1346,10 +1352,18 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="A36" s="1">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1358,24 +1372,20 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>20</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1398,20 +1408,24 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="A41" s="1">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1422,30 +1436,22 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>5</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1456,9 +1462,7 @@
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1468,22 +1472,30 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="A46" s="1">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1494,7 +1506,9 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -1539,6 +1553,42 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel Backlog & API
</commit_message>
<xml_diff>
--- a/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
+++ b/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web2.0\Documents\2-UsersStories\Propre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201742_students_ephec_be/Documents/0-COURS/BAC2/Q2/Dev_Info_Avance-Web/2-Projet/0-GitProjet_Gr29/Documents/2-UsersStories/Propre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E14F4AE-A93F-476F-AB81-9E938EBDEC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{0E14F4AE-A93F-476F-AB81-9E938EBDEC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B112C35D-8E08-824C-A77D-0EEE37BE6E2C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6BE69B5F-2B83-4C7C-919C-A491774D0366}"/>
+    <workbookView xWindow="28800" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{6BE69B5F-2B83-4C7C-919C-A491774D0366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t>Préparation</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>HTML</t>
-  </si>
-  <si>
     <t>connexion DB</t>
   </si>
   <si>
@@ -251,10 +248,64 @@
     <t>API</t>
   </si>
   <si>
-    <t>8h</t>
-  </si>
-  <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>4h30</t>
+  </si>
+  <si>
+    <t>1h00</t>
+  </si>
+  <si>
+    <t>7h00</t>
+  </si>
+  <si>
+    <t>9h00</t>
+  </si>
+  <si>
+    <t>5h00</t>
+  </si>
+  <si>
+    <t>Longue recherche pour la méthode POST</t>
+  </si>
+  <si>
+    <t>2h00</t>
+  </si>
+  <si>
+    <t>Sécurité</t>
+  </si>
+  <si>
+    <t>Tests Unitaires</t>
+  </si>
+  <si>
+    <t>GET init</t>
+  </si>
+  <si>
+    <t>GET login</t>
+  </si>
+  <si>
+    <t>GET eleves</t>
+  </si>
+  <si>
+    <t>GET garderie</t>
+  </si>
+  <si>
+    <t>GET elevesId</t>
+  </si>
+  <si>
+    <t>GET elevesName</t>
+  </si>
+  <si>
+    <t>GET parentsId</t>
+  </si>
+  <si>
+    <t>POST eleves</t>
+  </si>
+  <si>
+    <t>POST parents</t>
+  </si>
+  <si>
+    <t>POST garderie</t>
   </si>
 </sst>
 </file>
@@ -283,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +350,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -340,6 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,22 +712,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5B8967-943E-45FD-AD50-36B24B8571A1}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -695,7 +754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -707,7 +766,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -729,7 +788,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -751,7 +810,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -763,13 +822,15 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -782,16 +843,16 @@
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>51</v>
@@ -809,7 +870,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>53</v>
@@ -821,13 +882,15 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>55</v>
@@ -845,7 +908,7 @@
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>55</v>
@@ -863,13 +926,13 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -881,7 +944,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -893,10 +956,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -904,14 +967,16 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="J13" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -923,7 +988,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>100</v>
       </c>
@@ -931,7 +996,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -939,11 +1004,11 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>100</v>
       </c>
@@ -951,7 +1016,7 @@
         <v>61</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -959,11 +1024,11 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>100</v>
       </c>
@@ -971,21 +1036,19 @@
         <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="6" t="s">
         <v>58</v>
       </c>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -997,7 +1060,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>100</v>
       </c>
@@ -1019,7 +1082,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>100</v>
       </c>
@@ -1041,7 +1104,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>100</v>
       </c>
@@ -1063,7 +1126,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>100</v>
       </c>
@@ -1085,7 +1148,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>100</v>
       </c>
@@ -1103,11 +1166,13 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>100</v>
       </c>
@@ -1129,7 +1194,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>100</v>
       </c>
@@ -1137,109 +1202,113 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>100</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>68</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>80</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1247,21 +1316,21 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1269,7 +1338,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>50</v>
       </c>
@@ -1280,16 +1349,20 @@
         <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>50</v>
       </c>
@@ -1300,38 +1373,40 @@
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>5</v>
       </c>
@@ -1342,16 +1417,18 @@
         <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>5</v>
       </c>
@@ -1362,7 +1439,7 @@
         <v>27</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1371,11 +1448,19 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1383,7 +1468,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1395,7 +1480,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1407,7 +1492,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1419,14 +1504,14 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>20</v>
-      </c>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -1435,10 +1520,12 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1447,10 +1534,12 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -1459,10 +1548,12 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1471,31 +1562,27 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>5</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1503,11 +1590,11 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1517,10 +1604,12 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -1529,10 +1618,12 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1541,10 +1632,12 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="C50" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -1553,21 +1646,25 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>95</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1577,17 +1674,187 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>20</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Backlog Excel V2
</commit_message>
<xml_diff>
--- a/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
+++ b/Documents/2-UsersStories/Propre/BacklogExcel.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_9d4\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201742_students_ephec_be/Documents/0-COURS/BAC2/Q2/Dev_Info_Avance-Web/2-Projet/0-GitProjet_Gr29/Documents/2-UsersStories/Propre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="440" documentId="13_ncr:1_{0E14F4AE-A93F-476F-AB81-9E938EBDEC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{307A6634-0EE1-4659-9C53-F215E37B85EF}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="13_ncr:1_{0E14F4AE-A93F-476F-AB81-9E938EBDEC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AB442C2-D8B9-F244-BD09-9A8BA64EF942}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="435" windowWidth="33600" windowHeight="20565" xr2:uid="{6BE69B5F-2B83-4C7C-919C-A491774D0366}"/>
+    <workbookView xWindow="28800" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{6BE69B5F-2B83-4C7C-919C-A491774D0366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -484,7 +484,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -690,7 +690,7 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,7 +735,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1033,27 +1033,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5B8967-943E-45FD-AD50-36B24B8571A1}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="86.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="86.6640625" style="14" customWidth="1"/>
     <col min="6" max="6" width="44" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" style="14" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="38.5" style="14" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>138</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1101,7 +1101,7 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -1124,7 +1124,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -1147,7 +1147,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -1168,7 +1168,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -1191,7 +1191,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1210,7 +1210,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -1231,7 +1231,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
@@ -1269,7 +1269,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1288,7 +1288,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -1309,7 +1309,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -1322,7 +1322,7 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>100</v>
       </c>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>100</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>100</v>
       </c>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1412,7 +1412,7 @@
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>100</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>100</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>100</v>
       </c>
@@ -1503,7 +1503,7 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>100</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>100</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>100</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" ht="173.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="2" customFormat="1" ht="173" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>100</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -1640,7 +1640,7 @@
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>50</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>50</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>50</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1742,7 +1742,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1755,7 +1755,7 @@
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
     </row>
-    <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>50</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1797,7 +1797,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1810,7 +1810,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -1823,7 +1823,7 @@
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="23" t="s">
@@ -1840,7 +1840,7 @@
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="23" t="s">
@@ -1857,7 +1857,7 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="23" t="s">
@@ -1874,7 +1874,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="23" t="s">
@@ -1891,7 +1891,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="23" t="s">
@@ -1908,7 +1908,7 @@
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="23" t="s">
@@ -1925,7 +1925,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="23" t="s">
@@ -1942,7 +1942,7 @@
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="23" t="s">
@@ -1959,7 +1959,7 @@
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="23"/>
@@ -1972,7 +1972,7 @@
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="23" t="s">
@@ -1989,7 +1989,7 @@
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="23" t="s">
@@ -2006,7 +2006,7 @@
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="23" t="s">
@@ -2023,7 +2023,7 @@
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="23" t="s">
@@ -2040,7 +2040,7 @@
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="23" t="s">
@@ -2057,7 +2057,7 @@
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="23" t="s">
@@ -2074,7 +2074,7 @@
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="23" t="s">
@@ -2091,7 +2091,7 @@
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="23" t="s">
@@ -2108,7 +2108,7 @@
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="23" t="s">
@@ -2125,7 +2125,7 @@
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="23" t="s">
@@ -2142,7 +2142,7 @@
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="23"/>
@@ -2155,7 +2155,7 @@
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="23" t="s">
@@ -2174,7 +2174,7 @@
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="23" t="s">
@@ -2193,7 +2193,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="23" t="s">
@@ -2212,7 +2212,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="23" t="s">
@@ -2231,7 +2231,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="23"/>
@@ -2244,7 +2244,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="23"/>
@@ -2257,7 +2257,7 @@
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2270,7 +2270,7 @@
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2283,7 +2283,7 @@
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -2296,7 +2296,7 @@
       <c r="J63" s="22"/>
       <c r="K63" s="22"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>5</v>
       </c>
@@ -2317,7 +2317,7 @@
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
@@ -2334,7 +2334,7 @@
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>5</v>
       </c>
@@ -2357,7 +2357,7 @@
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>5</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>5</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>10</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>5</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>5</v>
       </c>
@@ -2462,18 +2462,18 @@
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I74" s="29">
-        <f>SUM(I2:I72)</f>
-        <v>0</v>
+        <f t="shared" ref="I74:K74" si="0">SUM(I2:I72)</f>
+        <v>1.1666666666666665</v>
       </c>
       <c r="J74" s="29">
-        <f>SUM(J2:J72)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.62847222222222221</v>
       </c>
       <c r="K74" s="29">
-        <f>SUM(K2:K72)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>